<commit_message>
Added one more test
</commit_message>
<xml_diff>
--- a/testData/personalDetails.xlsx
+++ b/testData/personalDetails.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>firstName</t>
   </si>
@@ -67,7 +67,7 @@
     <t>Gonzales</t>
   </si>
   <si>
-    <t>New Zealander</t>
+    <t>Mexican</t>
   </si>
   <si>
     <t>Married</t>
@@ -80,6 +80,24 @@
   </si>
   <si>
     <t>This is data driven test</t>
+  </si>
+  <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>rabbit</t>
+  </si>
+  <si>
+    <t>Bunny</t>
+  </si>
+  <si>
+    <t>American</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>This is another data driven test</t>
   </si>
 </sst>
 </file>
@@ -99,13 +117,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -139,38 +157,38 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -477,7 +495,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -496,7 +514,7 @@
     <col min="11" max="11" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="9" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="9" width="28.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -562,29 +580,73 @@
       <c r="F2" s="2">
         <v>5551652</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="3">
         <v>49616</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="6">
-        <v>31174</v>
+      <c r="J2" s="3">
+        <v>19600</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="5">
         <v>123</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="6">
+        <v>5515</v>
+      </c>
+      <c r="E3" s="6">
+        <v>3685</v>
+      </c>
+      <c r="F3" s="6">
+        <v>5551742</v>
+      </c>
+      <c r="G3" s="7">
+        <v>50500</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="7">
+        <v>14819</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="8">
+        <v>456</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>